<commit_message>
Adicionado inserção de dados automatica
Adicionado inserção de dados automatica
</commit_message>
<xml_diff>
--- a/Tenenbaum_Latitude_1_2_2/Arquivos_adicionais/temperatura_latitude.xlsx
+++ b/Tenenbaum_Latitude_1_2_2/Arquivos_adicionais/temperatura_latitude.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3162c0a97888194f/Documentos/GitHub/algoritmos/Tenenbaum_Latitude_1_2_2/Arquivos_adicionais/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="169" documentId="8_{770B8826-73A4-431D-B610-1015C9328ED3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2A0881A4-4AF6-499C-B40A-70DC0A421962}"/>
+  <xr:revisionPtr revIDLastSave="185" documentId="8_{770B8826-73A4-431D-B610-1015C9328ED3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0A6CDD43-A14F-4353-B0FE-603B33B0E6E0}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{05D25BB4-2697-4CF4-9A33-461F6C101D9D}"/>
+    <workbookView xWindow="30645" yWindow="1995" windowWidth="21600" windowHeight="11385" xr2:uid="{05D25BB4-2697-4CF4-9A33-461F6C101D9D}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -90,8 +90,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.00000000000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -410,9 +411,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -428,11 +426,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -443,15 +448,11 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="57">
+  <dxfs count="6">
     <dxf>
       <fill>
         <patternFill>
@@ -491,363 +492,6 @@
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4561,7 +4205,7 @@
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
-                      <c:formatCode>0.00</c:formatCode>
+                      <c:formatCode>0.00000000000</c:formatCode>
                       <c:ptCount val="36"/>
                       <c:pt idx="0">
                         <c:v>-46.175000000000004</c:v>
@@ -8556,7 +8200,7 @@
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
-                      <c:formatCode>0.00</c:formatCode>
+                      <c:formatCode>0.00000000000</c:formatCode>
                       <c:ptCount val="36"/>
                       <c:pt idx="0">
                         <c:v>-46.175000000000004</c:v>
@@ -10454,41 +10098,42 @@
   <dimension ref="B1:O40"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R37" sqref="R37"/>
+      <selection activeCell="T13" sqref="T13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="3" max="15" width="8.7109375" customWidth="1"/>
+    <col min="3" max="14" width="8.7109375" customWidth="1"/>
+    <col min="15" max="15" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="8.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="18" t="s">
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="16" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B3" s="17"/>
+      <c r="B3" s="19"/>
       <c r="C3" s="5" t="s">
         <v>2</v>
       </c>
@@ -10522,13 +10167,13 @@
       <c r="M3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="8" t="s">
+      <c r="N3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="O3" s="15"/>
+      <c r="O3" s="17"/>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="11">
+      <c r="B4" s="10">
         <v>-87.5</v>
       </c>
       <c r="C4" s="3">
@@ -10564,7 +10209,7 @@
       <c r="M4" s="1">
         <v>-35.700000000000003</v>
       </c>
-      <c r="N4" s="9">
+      <c r="N4" s="8">
         <v>-25.6</v>
       </c>
       <c r="O4" s="13">
@@ -10573,7 +10218,7 @@
       </c>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="11">
+      <c r="B5" s="10">
         <v>-82.5</v>
       </c>
       <c r="C5" s="3">
@@ -10609,7 +10254,7 @@
       <c r="M5" s="1">
         <v>-29.5</v>
       </c>
-      <c r="N5" s="9">
+      <c r="N5" s="8">
         <v>-20.399999999999999</v>
       </c>
       <c r="O5" s="13">
@@ -10618,7 +10263,7 @@
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B6" s="11">
+      <c r="B6" s="10">
         <v>-77.5</v>
       </c>
       <c r="C6" s="3">
@@ -10654,7 +10299,7 @@
       <c r="M6" s="1">
         <v>-26.3</v>
       </c>
-      <c r="N6" s="9">
+      <c r="N6" s="8">
         <v>-18</v>
       </c>
       <c r="O6" s="13">
@@ -10663,7 +10308,7 @@
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B7" s="11">
+      <c r="B7" s="10">
         <v>-72.5</v>
       </c>
       <c r="C7" s="3">
@@ -10699,7 +10344,7 @@
       <c r="M7" s="1">
         <v>-18.5</v>
       </c>
-      <c r="N7" s="9">
+      <c r="N7" s="8">
         <v>-12</v>
       </c>
       <c r="O7" s="13">
@@ -10708,7 +10353,7 @@
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B8" s="11">
+      <c r="B8" s="10">
         <v>-67.5</v>
       </c>
       <c r="C8" s="3">
@@ -10744,7 +10389,7 @@
       <c r="M8" s="1">
         <v>-7.2</v>
       </c>
-      <c r="N8" s="9">
+      <c r="N8" s="8">
         <v>-3.1</v>
       </c>
       <c r="O8" s="13">
@@ -10753,7 +10398,7 @@
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B9" s="11">
+      <c r="B9" s="10">
         <v>-62.5</v>
       </c>
       <c r="C9" s="3">
@@ -10789,7 +10434,7 @@
       <c r="M9" s="1">
         <v>-1.9</v>
       </c>
-      <c r="N9" s="9">
+      <c r="N9" s="8">
         <v>0.5</v>
       </c>
       <c r="O9" s="13">
@@ -10798,7 +10443,7 @@
       </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B10" s="11">
+      <c r="B10" s="10">
         <v>-57.5</v>
       </c>
       <c r="C10" s="3">
@@ -10834,7 +10479,7 @@
       <c r="M10" s="1">
         <v>1.1000000000000001</v>
       </c>
-      <c r="N10" s="9">
+      <c r="N10" s="8">
         <v>2.4</v>
       </c>
       <c r="O10" s="13">
@@ -10843,7 +10488,7 @@
       </c>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B11" s="11">
+      <c r="B11" s="10">
         <v>-52.5</v>
       </c>
       <c r="C11" s="3">
@@ -10879,7 +10524,7 @@
       <c r="M11" s="1">
         <v>4.0999999999999996</v>
       </c>
-      <c r="N11" s="9">
+      <c r="N11" s="8">
         <v>5.4</v>
       </c>
       <c r="O11" s="13">
@@ -10888,7 +10533,7 @@
       </c>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B12" s="11">
+      <c r="B12" s="10">
         <v>-47.5</v>
       </c>
       <c r="C12" s="3">
@@ -10924,7 +10569,7 @@
       <c r="M12" s="1">
         <v>7.4</v>
       </c>
-      <c r="N12" s="9">
+      <c r="N12" s="8">
         <v>8.6999999999999993</v>
       </c>
       <c r="O12" s="13">
@@ -10933,7 +10578,7 @@
       </c>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B13" s="11">
+      <c r="B13" s="10">
         <v>-42.5</v>
       </c>
       <c r="C13" s="3">
@@ -10969,7 +10614,7 @@
       <c r="M13" s="1">
         <v>11.3</v>
       </c>
-      <c r="N13" s="9">
+      <c r="N13" s="8">
         <v>12.6</v>
       </c>
       <c r="O13" s="13">
@@ -10978,7 +10623,7 @@
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B14" s="11">
+      <c r="B14" s="10">
         <v>-37.5</v>
       </c>
       <c r="C14" s="3">
@@ -11014,7 +10659,7 @@
       <c r="M14" s="1">
         <v>14.8</v>
       </c>
-      <c r="N14" s="9">
+      <c r="N14" s="8">
         <v>16.3</v>
       </c>
       <c r="O14" s="13">
@@ -11023,7 +10668,7 @@
       </c>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B15" s="11">
+      <c r="B15" s="10">
         <v>-32.5</v>
       </c>
       <c r="C15" s="3">
@@ -11059,7 +10704,7 @@
       <c r="M15" s="1">
         <v>17.8</v>
       </c>
-      <c r="N15" s="9">
+      <c r="N15" s="8">
         <v>19.600000000000001</v>
       </c>
       <c r="O15" s="13">
@@ -11068,7 +10713,7 @@
       </c>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B16" s="11">
+      <c r="B16" s="10">
         <v>-27.5</v>
       </c>
       <c r="C16" s="3">
@@ -11104,7 +10749,7 @@
       <c r="M16" s="1">
         <v>20.6</v>
       </c>
-      <c r="N16" s="9">
+      <c r="N16" s="8">
         <v>22.3</v>
       </c>
       <c r="O16" s="13">
@@ -11113,7 +10758,7 @@
       </c>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B17" s="11">
+      <c r="B17" s="10">
         <v>-22.5</v>
       </c>
       <c r="C17" s="3">
@@ -11149,7 +10794,7 @@
       <c r="M17" s="1">
         <v>22.8</v>
       </c>
-      <c r="N17" s="9">
+      <c r="N17" s="8">
         <v>23.9</v>
       </c>
       <c r="O17" s="13">
@@ -11158,7 +10803,7 @@
       </c>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B18" s="11">
+      <c r="B18" s="10">
         <v>-17.5</v>
       </c>
       <c r="C18" s="3">
@@ -11194,7 +10839,7 @@
       <c r="M18" s="1">
         <v>24.2</v>
       </c>
-      <c r="N18" s="9">
+      <c r="N18" s="8">
         <v>24.8</v>
       </c>
       <c r="O18" s="13">
@@ -11203,7 +10848,7 @@
       </c>
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B19" s="11">
+      <c r="B19" s="10">
         <v>-12.5</v>
       </c>
       <c r="C19" s="3">
@@ -11239,7 +10884,7 @@
       <c r="M19" s="1">
         <v>25</v>
       </c>
-      <c r="N19" s="9">
+      <c r="N19" s="8">
         <v>25.3</v>
       </c>
       <c r="O19" s="13">
@@ -11248,7 +10893,7 @@
       </c>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B20" s="11">
+      <c r="B20" s="10">
         <v>-7.5</v>
       </c>
       <c r="C20" s="3">
@@ -11284,7 +10929,7 @@
       <c r="M20" s="1">
         <v>25.7</v>
       </c>
-      <c r="N20" s="9">
+      <c r="N20" s="8">
         <v>25.8</v>
       </c>
       <c r="O20" s="13">
@@ -11293,7 +10938,7 @@
       </c>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B21" s="11">
+      <c r="B21" s="10">
         <v>-2.5</v>
       </c>
       <c r="C21" s="3">
@@ -11329,7 +10974,7 @@
       <c r="M21" s="1">
         <v>25.8</v>
       </c>
-      <c r="N21" s="9">
+      <c r="N21" s="8">
         <v>25.9</v>
       </c>
       <c r="O21" s="13">
@@ -11338,7 +10983,7 @@
       </c>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B22" s="11">
+      <c r="B22" s="10">
         <v>2.5</v>
       </c>
       <c r="C22" s="3">
@@ -11374,7 +11019,7 @@
       <c r="M22" s="1">
         <v>26.1</v>
       </c>
-      <c r="N22" s="9">
+      <c r="N22" s="8">
         <v>26</v>
       </c>
       <c r="O22" s="13">
@@ -11383,7 +11028,7 @@
       </c>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B23" s="11">
+      <c r="B23" s="10">
         <v>7.5</v>
       </c>
       <c r="C23" s="3">
@@ -11419,7 +11064,7 @@
       <c r="M23" s="1">
         <v>26.3</v>
       </c>
-      <c r="N23" s="9">
+      <c r="N23" s="8">
         <v>25.9</v>
       </c>
       <c r="O23" s="13">
@@ -11428,7 +11073,7 @@
       </c>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B24" s="11">
+      <c r="B24" s="10">
         <v>12.5</v>
       </c>
       <c r="C24" s="3">
@@ -11464,7 +11109,7 @@
       <c r="M24" s="1">
         <v>26.4</v>
       </c>
-      <c r="N24" s="9">
+      <c r="N24" s="8">
         <v>25.3</v>
       </c>
       <c r="O24" s="13">
@@ -11473,7 +11118,7 @@
       </c>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B25" s="11">
+      <c r="B25" s="10">
         <v>17.5</v>
       </c>
       <c r="C25" s="3">
@@ -11509,7 +11154,7 @@
       <c r="M25" s="1">
         <v>25.2</v>
       </c>
-      <c r="N25" s="9">
+      <c r="N25" s="8">
         <v>23.6</v>
       </c>
       <c r="O25" s="13">
@@ -11518,7 +11163,7 @@
       </c>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B26" s="11">
+      <c r="B26" s="10">
         <v>22.5</v>
       </c>
       <c r="C26" s="3">
@@ -11554,7 +11199,7 @@
       <c r="M26" s="1">
         <v>23.1</v>
       </c>
-      <c r="N26" s="9">
+      <c r="N26" s="8">
         <v>20.8</v>
       </c>
       <c r="O26" s="13">
@@ -11563,7 +11208,7 @@
       </c>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B27" s="11">
+      <c r="B27" s="10">
         <v>27.5</v>
       </c>
       <c r="C27" s="3">
@@ -11599,7 +11244,7 @@
       <c r="M27" s="1">
         <v>19.7</v>
       </c>
-      <c r="N27" s="9">
+      <c r="N27" s="8">
         <v>16.7</v>
       </c>
       <c r="O27" s="13">
@@ -11608,7 +11253,7 @@
       </c>
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B28" s="11">
+      <c r="B28" s="10">
         <v>32.5</v>
       </c>
       <c r="C28" s="3">
@@ -11644,7 +11289,7 @@
       <c r="M28" s="1">
         <v>15</v>
       </c>
-      <c r="N28" s="9">
+      <c r="N28" s="8">
         <v>11.7</v>
       </c>
       <c r="O28" s="13">
@@ -11653,7 +11298,7 @@
       </c>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B29" s="11">
+      <c r="B29" s="10">
         <v>37.5</v>
       </c>
       <c r="C29" s="3">
@@ -11689,7 +11334,7 @@
       <c r="M29" s="1">
         <v>11</v>
       </c>
-      <c r="N29" s="9">
+      <c r="N29" s="8">
         <v>7.1</v>
       </c>
       <c r="O29" s="13">
@@ -11698,7 +11343,7 @@
       </c>
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B30" s="11">
+      <c r="B30" s="10">
         <v>42.5</v>
       </c>
       <c r="C30" s="3">
@@ -11734,7 +11379,7 @@
       <c r="M30" s="1">
         <v>6.8</v>
       </c>
-      <c r="N30" s="9">
+      <c r="N30" s="8">
         <v>2.5</v>
       </c>
       <c r="O30" s="13">
@@ -11743,7 +11388,7 @@
       </c>
     </row>
     <row r="31" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B31" s="11">
+      <c r="B31" s="10">
         <v>47.5</v>
       </c>
       <c r="C31" s="3">
@@ -11779,7 +11424,7 @@
       <c r="M31" s="1">
         <v>2</v>
       </c>
-      <c r="N31" s="9">
+      <c r="N31" s="8">
         <v>-2.6</v>
       </c>
       <c r="O31" s="13">
@@ -11788,7 +11433,7 @@
       </c>
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B32" s="11">
+      <c r="B32" s="10">
         <v>52.5</v>
       </c>
       <c r="C32" s="3">
@@ -11824,7 +11469,7 @@
       <c r="M32" s="1">
         <v>-1.7</v>
       </c>
-      <c r="N32" s="9">
+      <c r="N32" s="8">
         <v>-6.7</v>
       </c>
       <c r="O32" s="13">
@@ -11833,7 +11478,7 @@
       </c>
     </row>
     <row r="33" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B33" s="11">
+      <c r="B33" s="10">
         <v>57.5</v>
       </c>
       <c r="C33" s="3">
@@ -11869,7 +11514,7 @@
       <c r="M33" s="1">
         <v>-4.8</v>
       </c>
-      <c r="N33" s="9">
+      <c r="N33" s="8">
         <v>-10</v>
       </c>
       <c r="O33" s="13">
@@ -11878,7 +11523,7 @@
       </c>
     </row>
     <row r="34" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B34" s="11">
+      <c r="B34" s="10">
         <v>62.5</v>
       </c>
       <c r="C34" s="3">
@@ -11914,7 +11559,7 @@
       <c r="M34" s="1">
         <v>-12.3</v>
       </c>
-      <c r="N34" s="9">
+      <c r="N34" s="8">
         <v>-17.8</v>
       </c>
       <c r="O34" s="13">
@@ -11923,7 +11568,7 @@
       </c>
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B35" s="11">
+      <c r="B35" s="10">
         <v>67.5</v>
       </c>
       <c r="C35" s="3">
@@ -11959,7 +11604,7 @@
       <c r="M35" s="1">
         <v>-17.2</v>
       </c>
-      <c r="N35" s="9">
+      <c r="N35" s="8">
         <v>-22.2</v>
       </c>
       <c r="O35" s="13">
@@ -11968,7 +11613,7 @@
       </c>
     </row>
     <row r="36" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B36" s="11">
+      <c r="B36" s="10">
         <v>72.5</v>
       </c>
       <c r="C36" s="3">
@@ -12004,7 +11649,7 @@
       <c r="M36" s="1">
         <v>-19.399999999999999</v>
       </c>
-      <c r="N36" s="9">
+      <c r="N36" s="8">
         <v>-23.6</v>
       </c>
       <c r="O36" s="13">
@@ -12013,7 +11658,7 @@
       </c>
     </row>
     <row r="37" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B37" s="11">
+      <c r="B37" s="10">
         <v>77.5</v>
       </c>
       <c r="C37" s="3">
@@ -12049,7 +11694,7 @@
       <c r="M37" s="1">
         <v>-22.1</v>
       </c>
-      <c r="N37" s="9">
+      <c r="N37" s="8">
         <v>-26</v>
       </c>
       <c r="O37" s="13">
@@ -12058,7 +11703,7 @@
       </c>
     </row>
     <row r="38" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B38" s="11">
+      <c r="B38" s="10">
         <v>82.5</v>
       </c>
       <c r="C38" s="3">
@@ -12094,7 +11739,7 @@
       <c r="M38" s="1">
         <v>-24</v>
       </c>
-      <c r="N38" s="9">
+      <c r="N38" s="8">
         <v>-28.1</v>
       </c>
       <c r="O38" s="13">
@@ -12103,7 +11748,7 @@
       </c>
     </row>
     <row r="39" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="12">
+      <c r="B39" s="11">
         <v>87.5</v>
       </c>
       <c r="C39" s="4">
@@ -12139,7 +11784,7 @@
       <c r="M39" s="2">
         <v>-24.7</v>
       </c>
-      <c r="N39" s="10">
+      <c r="N39" s="9">
         <v>-29.2</v>
       </c>
       <c r="O39" s="14">
@@ -12148,19 +11793,19 @@
       </c>
     </row>
     <row r="40" spans="2:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C40" s="19"/>
-      <c r="D40" s="19"/>
-      <c r="E40" s="19"/>
-      <c r="F40" s="19"/>
-      <c r="G40" s="19"/>
-      <c r="H40" s="19"/>
-      <c r="I40" s="19"/>
-      <c r="J40" s="19"/>
-      <c r="K40" s="19"/>
-      <c r="L40" s="19"/>
-      <c r="M40" s="19"/>
-      <c r="N40" s="19"/>
-      <c r="O40" s="19"/>
+      <c r="C40" s="12"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="12"/>
+      <c r="F40" s="12"/>
+      <c r="G40" s="12"/>
+      <c r="H40" s="12"/>
+      <c r="I40" s="12"/>
+      <c r="J40" s="12"/>
+      <c r="K40" s="12"/>
+      <c r="L40" s="12"/>
+      <c r="M40" s="12"/>
+      <c r="N40" s="12"/>
+      <c r="O40" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>